<commit_message>
changes in filter_tags file
</commit_message>
<xml_diff>
--- a/filter_tags.xlsx
+++ b/filter_tags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgenstensrud/Documents/tags_creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4633F2EC-7738-AD43-BD42-A45356D113ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28A7D30-2669-E749-B058-81BECA09B7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="500" windowWidth="34560" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51680" yWindow="-2600" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -152,12 +152,6 @@
     <t>Naval</t>
   </si>
   <si>
-    <t>3D sonar technology, advanced navigation system, HISAS, Sunstone,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sub-bottom profiler, Multibeam sonar, Side Scan Sonar, Single beam echo sounder, </t>
-  </si>
-  <si>
     <t>Modem, Radio, subsea, surface, transceiver</t>
   </si>
   <si>
@@ -192,6 +186,12 @@
   </si>
   <si>
     <t>GPS, vessel tracking, maritime navigation, environmental monitoring</t>
+  </si>
+  <si>
+    <t>3D sonar technology, advanced navigation system, HISAS, Sunstone</t>
+  </si>
+  <si>
+    <t>Sub-bottom profiler, Multibeam sonar, Side Scan Sonar, Single beam echo sounder</t>
   </si>
 </sst>
 </file>
@@ -558,7 +558,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="F24" sqref="B24:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -574,7 +574,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -588,7 +588,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -630,7 +630,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -644,10 +644,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
         <v>50</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -658,13 +658,13 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -689,7 +689,7 @@
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
         <v>28</v>
@@ -703,10 +703,10 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -714,10 +714,10 @@
         <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
         <v>32</v>
@@ -742,7 +742,7 @@
         <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>

</xml_diff>